<commit_message>
deep learning model applied
</commit_message>
<xml_diff>
--- a/results/StereoCAMDistance.xlsx
+++ b/results/StereoCAMDistance.xlsx
@@ -1,21 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JTech\Passive-Stereo-CAM-Distance\results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
-  </bookViews>
   <sheets>
-    <sheet name="Dataset" sheetId="1" r:id="rId1"/>
-    <sheet name="prediction" sheetId="2" r:id="rId2"/>
+    <sheet state="visible" name="Dataset" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="prediction" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
@@ -37,16 +29,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="2">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -57,47 +48,32 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="2"/>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
       <c:tx>
@@ -114,7 +90,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="0">
+              <a:rPr b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -125,14 +101,11 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -140,12 +113,6 @@
           <c:tx>
             <c:strRef>
               <c:f>Dataset!$A$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>distance</c:v>
-                </c:pt>
-              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -177,6 +144,7 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
+            <c:name/>
             <c:spPr>
               <a:ln w="19050">
                 <a:solidFill>
@@ -189,136 +157,20 @@
             <c:trendlineType val="exp"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
           </c:trendline>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Dataset!$B$2:$B$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>0.98</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.82</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.67</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.54</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.43</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.28000000000000003</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.26</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7.0000000000000007E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Dataset!$A$2:$A$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9753-4907-9037-F1A3ECE904DE}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
         <c:axId val="138654365"/>
         <c:axId val="1558477603"/>
       </c:lineChart>
@@ -344,7 +196,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" b="0">
+                  <a:rPr b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -355,13 +207,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:spPr/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -374,21 +225,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1558477603"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="1558477603"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="300"/>
+          <c:max val="300.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -427,7 +272,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" b="0">
+                  <a:rPr b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -438,7 +283,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -460,17 +304,13 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="138654365"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -484,28 +324,16 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="2"/>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
       <c:tx>
@@ -522,7 +350,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="0">
+              <a:rPr b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -533,31 +361,21 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
               <c:f>prediction!$A$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Acutal distance</c:v>
-                </c:pt>
-              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cmpd="sng">
+            <a:ln cmpd="sng" w="19050">
               <a:solidFill>
                 <a:srgbClr val="4285F4"/>
               </a:solidFill>
@@ -580,51 +398,10 @@
           <c:val>
             <c:numRef>
               <c:f>prediction!$A$2:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>160</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C3D3-4BF7-AAB4-9DEFF4BBD8B2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -632,16 +409,10 @@
           <c:tx>
             <c:strRef>
               <c:f>prediction!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>predicted distance</c:v>
-                </c:pt>
-              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cmpd="sng">
+            <a:ln cmpd="sng" w="19050">
               <a:solidFill>
                 <a:srgbClr val="EA4335"/>
               </a:solidFill>
@@ -664,62 +435,11 @@
           <c:val>
             <c:numRef>
               <c:f>prediction!$B$2:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>122</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>137</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>143</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>156</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C3D3-4BF7-AAB4-9DEFF4BBD8B2}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
         <c:axId val="1422869559"/>
         <c:axId val="113192072"/>
       </c:lineChart>
@@ -744,17 +464,24 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:spPr/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -767,15 +494,9 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="113192072"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="113192072"/>
@@ -818,11 +539,18 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -844,17 +572,13 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1422869559"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -868,35 +592,27 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6324600" cy="3524250"/>
-    <xdr:graphicFrame macro="">
+    <xdr:ext cx="8915400" cy="5514975"/>
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1" title="Chart"/>
+        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -905,7 +621,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -915,16 +631,16 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
@@ -935,7 +651,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -945,7 +661,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1135,25 +851,20 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1161,150 +872,142 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1">
-        <v>30</v>
+        <v>30.0</v>
       </c>
       <c r="B2" s="1">
         <v>0.98</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1">
-        <v>40</v>
+        <v>40.0</v>
       </c>
       <c r="B3" s="1">
         <v>0.85</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1">
-        <v>45</v>
+        <v>45.0</v>
       </c>
       <c r="B4" s="1">
         <v>0.82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1">
-        <v>50</v>
+        <v>50.0</v>
       </c>
       <c r="B5" s="1">
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1">
-        <v>55</v>
+        <v>55.0</v>
       </c>
       <c r="B6" s="1">
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1">
-        <v>60</v>
+        <v>60.0</v>
       </c>
       <c r="B7" s="1">
         <v>0.67</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1">
-        <v>65</v>
+        <v>65.0</v>
       </c>
       <c r="B8" s="1">
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1">
-        <v>70</v>
+        <v>70.0</v>
       </c>
       <c r="B9" s="1">
         <v>0.54</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1">
-        <v>75</v>
+        <v>75.0</v>
       </c>
       <c r="B10" s="1">
         <v>0.43</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1">
-        <v>80</v>
+        <v>80.0</v>
       </c>
       <c r="B11" s="1">
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1">
-        <v>85</v>
+        <v>85.0</v>
       </c>
       <c r="B12" s="1">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.28</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" s="1">
-        <v>90</v>
+        <v>90.0</v>
       </c>
       <c r="B13" s="1">
         <v>0.26</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="B14" s="1">
         <v>0.13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1">
-        <v>110</v>
+        <v>110.0</v>
       </c>
       <c r="B15" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.07</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28" s="1">
-        <v>300</v>
+        <v>300.0</v>
       </c>
       <c r="B28" s="1">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1312,96 +1015,95 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1">
-        <v>60</v>
+        <v>60.0</v>
       </c>
       <c r="B2" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="1">
-        <v>70</v>
+        <v>70.0</v>
       </c>
       <c r="B3" s="1">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>72.0</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1">
-        <v>80</v>
+        <v>80.0</v>
       </c>
       <c r="B4" s="1">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>84.0</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="1">
-        <v>90</v>
+        <v>90.0</v>
       </c>
       <c r="B5" s="1">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>93.0</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="1">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="B6" s="1">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>110.0</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="1">
-        <v>110</v>
+        <v>110.0</v>
       </c>
       <c r="B7" s="1">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>115.0</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" s="1">
-        <v>120</v>
+        <v>120.0</v>
       </c>
       <c r="B8" s="1">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>113.0</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" s="1">
-        <v>130</v>
+        <v>130.0</v>
       </c>
       <c r="B9" s="1">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>122.0</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="1">
-        <v>140</v>
+        <v>140.0</v>
       </c>
       <c r="B10" s="1">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>137.0</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" s="1">
-        <v>150</v>
+        <v>150.0</v>
       </c>
       <c r="B11" s="1">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>143.0</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" s="1">
-        <v>160</v>
+        <v>160.0</v>
       </c>
       <c r="B12" s="1">
-        <v>156</v>
+        <v>156.0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>